<commit_message>
Add intermediate data & prompts & update existing adata - Add intermediate data - Overlaying of existing data (colors and lines) - Add prompts
</commit_message>
<xml_diff>
--- a/output/PHPCourses/PHPCourses-Clusters-S=H-B=1.00-k=8.xlsx
+++ b/output/PHPCourses/PHPCourses-Clusters-S=H-B=1.00-k=8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\metalman\Desktop\git\CREA-GPT5-CaseStudy-Results\output\PHPCourses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E03089A-F1A6-4419-80F3-03E5CBB96F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2F2713-6AEA-4039-8C1C-98D6B6DE47E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,15 +105,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -121,19 +133,121 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -426,10 +540,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
     </row>
@@ -437,13 +551,13 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -451,13 +565,13 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -465,13 +579,13 @@
       <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -479,13 +593,13 @@
       <c r="A8" s="1">
         <v>4</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -493,13 +607,13 @@
       <c r="A10" s="1">
         <v>5</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -507,13 +621,13 @@
       <c r="A12" s="1">
         <v>6</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -521,13 +635,13 @@
       <c r="A14" s="1">
         <v>7</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -535,17 +649,27 @@
       <c r="A16" s="1">
         <v>8</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="3" t="s">
+    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
+      <c r="B17" s="4" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>